<commit_message>
Initial publish: quotation app
</commit_message>
<xml_diff>
--- a/data/records.xlsx
+++ b/data/records.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -633,7 +633,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>20251116-006</t>
+          <t>20251116-002</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -643,33 +643,62 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>R-20251116-20251116-002-1</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Fahad Ahmed Mohammed</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Abu Dhabi - Al Shamkha</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>20251116-007</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025-11-16</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>q</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>QUO-20251116-001</t>
         </is>
       </c>
-      <c r="E6" t="n">
-        <v>3300</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Fahad Ahmed Mohamed</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>0502992932</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
+      <c r="E7" t="n">
+        <v>4680</v>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
         <is>
           <t>Abu Dhabi - Al Shamkha</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: add {{QTY}} placeholder and center alignment in Word export for quotation
</commit_message>
<xml_diff>
--- a/data/records.xlsx
+++ b/data/records.xlsx
@@ -1445,7 +1445,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>20251121-004</t>
+          <t>20251121-005</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1460,11 +1460,11 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>QUO-20251121-004</t>
+          <t>QUO-20251121-003</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>435</v>
+        <v>580</v>
       </c>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
@@ -1493,11 +1493,11 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>QUO-20251121-003</t>
+          <t>QUO-20251121-005</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>580</v>
+        <v>1015</v>
       </c>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
@@ -1511,7 +1511,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>20251121-005</t>
+          <t>20251121-007</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1526,7 +1526,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>QUO-20251121-005</t>
+          <t>QUO-20251121-008</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -1559,11 +1559,11 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>QUO-20251121-008</t>
+          <t>QUO-20251121-001</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>1015</v>
+        <v>7540</v>
       </c>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
@@ -1592,11 +1592,11 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>QUO-20251121-001</t>
+          <t>QUO-20251121-004</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>580</v>
+        <v>7540</v>
       </c>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>

</xml_diff>